<commit_message>
Send email with Queue & Bull
</commit_message>
<xml_diff>
--- a/xlsx-template/attch-email.xlsx
+++ b/xlsx-template/attch-email.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\vyvu\comartek-training\student-manager\xlsx-template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\vyvu\comartek-training\student-manager-mongo\xlsx-template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,27 +24,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Điểm môn ${subject.name} đã được cập nhật</t>
   </si>
   <si>
-    <t>studentId</t>
-  </si>
-  <si>
     <t>studentName</t>
   </si>
   <si>
-    <t>${student.id}</t>
-  </si>
-  <si>
     <t>${student.name}</t>
-  </si>
-  <si>
-    <t>subjectId</t>
-  </si>
-  <si>
-    <t>${subject.id}</t>
   </si>
   <si>
     <t>subjectName</t>
@@ -63,9 +51,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -120,15 +105,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -413,7 +398,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,11 +414,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
       <c r="F1" s="2"/>
@@ -445,16 +430,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -462,43 +441,37 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>